<commit_message>
add a hoops bot
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\root\telegram_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B485FD70-D2AE-410B-8B69-BC4A918FBAE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B6BC0A-CBFC-4200-80A9-9A11CD647245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36090" yWindow="1335" windowWidth="21510" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t xml:space="preserve">שם משפחה </t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>נועם</t>
+  </si>
+  <si>
+    <t>פרץ</t>
+  </si>
+  <si>
+    <t>דביר</t>
+  </si>
+  <si>
+    <t>0545885537</t>
   </si>
 </sst>
 </file>
@@ -385,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,6 +461,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>